<commit_message>
VI:Modification in Login Page and Employee module
</commit_message>
<xml_diff>
--- a/RetentionTool/RetentionTool/Uploads/EmployeeDetails_DemoTest.xlsx
+++ b/RetentionTool/RetentionTool/Uploads/EmployeeDetails_DemoTest.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Promantus Inc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Projects\ResourceRetentionTool\RetentionTool\RetentionTool\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D563FE8-2A90-4A7A-A5C7-56D3A7482353}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7245" xr2:uid="{3BE88E27-7389-445B-AB1A-21220141C10B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16416" windowHeight="7248"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>21008</t>
   </si>
@@ -343,11 +342,14 @@
   <si>
     <t>Accounts</t>
   </si>
+  <si>
+    <t>Image</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -411,12 +413,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -724,19 +755,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B721820-F5AB-4721-9B34-F0137CD03EE2}">
-  <dimension ref="A1:P12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -785,8 +817,11 @@
       <c r="P1" s="5" t="s">
         <v>87</v>
       </c>
+      <c r="Q1" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -822,7 +857,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -855,7 +890,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -888,7 +923,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -932,7 +967,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -965,7 +1000,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -998,7 +1033,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1031,7 +1066,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1064,7 +1099,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1097,7 +1132,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="270" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1141,7 +1176,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="375" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="360" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1184,5 +1219,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>